<commit_message>
Alteração de graficos e cores
</commit_message>
<xml_diff>
--- a/CO2.xlsx
+++ b/CO2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marib\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263d74c401730189/Desktop/Power_BI_CO2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B823C857-654E-4364-81CA-EE2F31B38BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{B823C857-654E-4364-81CA-EE2F31B38BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{782B1B6C-E0DA-4302-9BC1-2B3696B86D6A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA6470DB-2E50-4B06-9BBF-07E65F96CCD6}"/>
+    <workbookView minimized="1" xWindow="15765" yWindow="1725" windowWidth="12705" windowHeight="11295" xr2:uid="{FA6470DB-2E50-4B06-9BBF-07E65F96CCD6}"/>
   </bookViews>
   <sheets>
     <sheet name="World_GDP_Population_CO2_Emissi" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -556,8 +556,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -606,13 +606,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -632,12 +632,12 @@
   <autoFilter ref="A1:K47" xr:uid="{CF1D4450-E042-4614-B209-6650D4CAFC6C}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2A5CB00D-5DCF-4192-B504-BA45BE231A93}" name="Year"/>
-    <tableColumn id="2" xr3:uid="{6640ED07-F5F0-4630-846C-31A7C1A402DD}" name="GDP Real (USD) " dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{C6564623-741B-418A-AC99-BC41E3B8015E}" name="GDP growth (%)" dataDxfId="0" dataCellStyle="Porcentagem"/>
+    <tableColumn id="2" xr3:uid="{6640ED07-F5F0-4630-846C-31A7C1A402DD}" name="GDP Real (USD) " dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C6564623-741B-418A-AC99-BC41E3B8015E}" name="GDP growth (%)" dataDxfId="1" dataCellStyle="Porcentagem"/>
     <tableColumn id="4" xr3:uid="{35573A17-C0C7-4618-A378-923C1071D57D}" name="Per Capita"/>
     <tableColumn id="5" xr3:uid="{11F7026A-9F42-4CA5-A6BC-B7C207A3742B}" name="World Population"/>
     <tableColumn id="6" xr3:uid="{DD658468-AD93-49CA-A491-24DCB71C41B7}" name="Net Change"/>
-    <tableColumn id="7" xr3:uid="{3D54B6A2-7CD9-4094-9088-82BDA12AE372}" name="Population change (%)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{3D54B6A2-7CD9-4094-9088-82BDA12AE372}" name="Population change (%)" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{E5FDC992-64F7-4F4B-B4C0-DFB45EE2235A}" name="Fossil CO2 Emissions (tons)"/>
     <tableColumn id="9" xr3:uid="{74B537A2-9B12-451F-B835-10FB840A8362}" name="CO2 emissions change"/>
     <tableColumn id="10" xr3:uid="{F554F5FB-718E-4104-9A21-BCA669EB7A0C}" name="CO2 emissions per capita"/>
@@ -967,11 +967,12 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
@@ -1020,13 +1021,13 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2022</v>
+      <c r="A2" s="3">
+        <v>44562</v>
       </c>
       <c r="B2" s="1">
         <v>90800000000000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>3.2399999999999996E-4</v>
       </c>
       <c r="D2">
@@ -1038,7 +1039,7 @@
       <c r="F2">
         <v>66958801</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>8.3999999999999995E-3</v>
       </c>
       <c r="H2">
@@ -1055,13 +1056,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2021</v>
+      <c r="A3" s="3">
+        <v>44197</v>
       </c>
       <c r="B3" s="1">
         <v>87900000000000</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>6.3500000000000004E-4</v>
       </c>
       <c r="D3">
@@ -1073,7 +1074,7 @@
       <c r="F3">
         <v>67447099</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>8.6E-3</v>
       </c>
       <c r="H3">
@@ -1090,13 +1091,13 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2020</v>
+      <c r="A4" s="3">
+        <v>43831</v>
       </c>
       <c r="B4" s="1">
         <v>82700000000000</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>-2.8800000000000001E-4</v>
       </c>
       <c r="D4">
@@ -1108,7 +1109,7 @@
       <c r="F4">
         <v>75707594</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="H4">
@@ -1125,13 +1126,13 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2019</v>
+      <c r="A5" s="3">
+        <v>43466</v>
       </c>
       <c r="B5" s="1">
         <v>85100000000000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2.6800000000000001E-4</v>
       </c>
       <c r="D5">
@@ -1143,7 +1144,7 @@
       <c r="F5">
         <v>81390917</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="H5">
@@ -1160,13 +1161,13 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2018</v>
+      <c r="A6" s="3">
+        <v>43101</v>
       </c>
       <c r="B6" s="1">
         <v>82900000000000</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>3.28E-4</v>
       </c>
       <c r="D6">
@@ -1178,7 +1179,7 @@
       <c r="F6">
         <v>84284827</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="H6">
@@ -1195,13 +1196,13 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2017</v>
+      <c r="A7" s="3">
+        <v>42736</v>
       </c>
       <c r="B7" s="1">
         <v>80300000000000</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>3.4500000000000004E-4</v>
       </c>
       <c r="D7">
@@ -1213,7 +1214,7 @@
       <c r="F7">
         <v>87063428</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>1.15E-2</v>
       </c>
       <c r="H7">
@@ -1230,13 +1231,13 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
+      <c r="A8" s="3">
+        <v>42370</v>
       </c>
       <c r="B8" s="1">
         <v>77600000000000</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>2.81E-4</v>
       </c>
       <c r="D8">
@@ -1248,7 +1249,7 @@
       <c r="F8">
         <v>88062654</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>1.18E-2</v>
       </c>
       <c r="H8">
@@ -1265,13 +1266,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2015</v>
+      <c r="A9" s="3">
+        <v>42005</v>
       </c>
       <c r="B9" s="1">
         <v>75500000000000</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>3.1300000000000002E-4</v>
       </c>
       <c r="D9">
@@ -1283,7 +1284,7 @@
       <c r="F9">
         <v>88875628</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>1.2E-2</v>
       </c>
       <c r="H9">
@@ -1300,13 +1301,13 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2014</v>
+      <c r="A10" s="3">
+        <v>41640</v>
       </c>
       <c r="B10" s="1">
         <v>73200000000000</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>3.1300000000000002E-4</v>
       </c>
       <c r="D10">
@@ -1318,7 +1319,7 @@
       <c r="F10">
         <v>89822659</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>1.23E-2</v>
       </c>
       <c r="H10">
@@ -1335,13 +1336,13 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2013</v>
+      <c r="A11" s="3">
+        <v>41275</v>
       </c>
       <c r="B11" s="1">
         <v>71000000000000</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>2.8699999999999998E-4</v>
       </c>
       <c r="D11">
@@ -1353,7 +1354,7 @@
       <c r="F11">
         <v>90591100</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>1.26E-2</v>
       </c>
       <c r="H11">
@@ -1370,13 +1371,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2012</v>
+      <c r="A12" s="3">
+        <v>40909</v>
       </c>
       <c r="B12" s="1">
         <v>69000000000000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>2.6899999999999998E-4</v>
       </c>
       <c r="D12">
@@ -1388,7 +1389,7 @@
       <c r="F12">
         <v>90278720</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="H12">
@@ -1405,13 +1406,13 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2011</v>
+      <c r="A13" s="3">
+        <v>40544</v>
       </c>
       <c r="B13" s="1">
         <v>67200000000000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>3.3399999999999999E-4</v>
       </c>
       <c r="D13">
@@ -1423,7 +1424,7 @@
       <c r="F13">
         <v>89191617</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="H13">
@@ -1440,13 +1441,13 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2010</v>
+      <c r="A14" s="3">
+        <v>40179</v>
       </c>
       <c r="B14" s="1">
         <v>65000000000000</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>4.5199999999999998E-4</v>
       </c>
       <c r="D14">
@@ -1458,7 +1459,7 @@
       <c r="F14">
         <v>88965732</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>1.2800000000000001E-2</v>
       </c>
       <c r="H14">
@@ -1475,13 +1476,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2009</v>
+      <c r="A15" s="3">
+        <v>39814</v>
       </c>
       <c r="B15" s="1">
         <v>62200000000000</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>-1.34E-4</v>
       </c>
       <c r="D15">
@@ -1493,7 +1494,7 @@
       <c r="F15">
         <v>88308754</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>1.29E-2</v>
       </c>
       <c r="H15">
@@ -1510,13 +1511,13 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2008</v>
+      <c r="A16" s="3">
+        <v>39448</v>
       </c>
       <c r="B16" s="1">
         <v>63000000000000</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>2.0599999999999999E-4</v>
       </c>
       <c r="D16">
@@ -1528,7 +1529,7 @@
       <c r="F16">
         <v>87148881</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>1.29E-2</v>
       </c>
       <c r="H16">
@@ -1545,13 +1546,13 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2007</v>
+      <c r="A17" s="3">
+        <v>39083</v>
       </c>
       <c r="B17" s="1">
         <v>61800000000000</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>4.3700000000000005E-4</v>
       </c>
       <c r="D17">
@@ -1563,7 +1564,7 @@
       <c r="F17">
         <v>85856766</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>1.29E-2</v>
       </c>
       <c r="H17">
@@ -1580,13 +1581,13 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2006</v>
+      <c r="A18" s="3">
+        <v>38718</v>
       </c>
       <c r="B18" s="1">
         <v>59200000000000</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>4.46E-4</v>
       </c>
       <c r="D18">
@@ -1598,7 +1599,7 @@
       <c r="F18">
         <v>84481883</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>1.2800000000000001E-2</v>
       </c>
       <c r="H18">
@@ -1615,13 +1616,13 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2005</v>
+      <c r="A19" s="3">
+        <v>38353</v>
       </c>
       <c r="B19" s="1">
         <v>56700000000000</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>4.0200000000000001E-4</v>
       </c>
       <c r="D19">
@@ -1633,7 +1634,7 @@
       <c r="F19">
         <v>83592360</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>1.29E-2</v>
       </c>
       <c r="H19">
@@ -1650,13 +1651,13 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2004</v>
+      <c r="A20" s="3">
+        <v>37987</v>
       </c>
       <c r="B20" s="1">
         <v>54500000000000</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>4.4699999999999997E-4</v>
       </c>
       <c r="D20">
@@ -1668,7 +1669,7 @@
       <c r="F20">
         <v>83016138</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>1.29E-2</v>
       </c>
       <c r="H20">
@@ -1685,13 +1686,13 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2003</v>
+      <c r="A21" s="3">
+        <v>37622</v>
       </c>
       <c r="B21" s="1">
         <v>52100000000000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>3.0900000000000003E-4</v>
       </c>
       <c r="D21">
@@ -1703,7 +1704,7 @@
       <c r="F21">
         <v>82631292</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="H21">
@@ -1720,13 +1721,13 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2002</v>
+      <c r="A22" s="3">
+        <v>37257</v>
       </c>
       <c r="B22" s="1">
         <v>50600000000000</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>2.3199999999999997E-4</v>
       </c>
       <c r="D22">
@@ -1738,7 +1739,7 @@
       <c r="F22">
         <v>82793883</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22">
         <v>1.32E-2</v>
       </c>
       <c r="H22">
@@ -1755,13 +1756,13 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2001</v>
+      <c r="A23" s="3">
+        <v>36892</v>
       </c>
       <c r="B23" s="1">
         <v>49400000000000</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>2.0299999999999997E-4</v>
       </c>
       <c r="D23">
@@ -1773,7 +1774,7 @@
       <c r="F23">
         <v>83233466</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23">
         <v>1.35E-2</v>
       </c>
       <c r="H23">
@@ -1790,13 +1791,13 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2000</v>
+      <c r="A24" s="3">
+        <v>36526</v>
       </c>
       <c r="B24" s="1">
         <v>48400000000000</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>4.5300000000000001E-4</v>
       </c>
       <c r="D24">
@@ -1808,7 +1809,7 @@
       <c r="F24">
         <v>82696654</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24">
         <v>1.3599999999999999E-2</v>
       </c>
       <c r="H24">
@@ -1825,13 +1826,13 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1999</v>
+      <c r="A25" s="3">
+        <v>36161</v>
       </c>
       <c r="B25" s="1">
         <v>46300000000000</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>3.59E-4</v>
       </c>
       <c r="D25">
@@ -1843,7 +1844,7 @@
       <c r="F25">
         <v>81939649</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25">
         <v>1.3599999999999999E-2</v>
       </c>
       <c r="H25">
@@ -1860,13 +1861,13 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1998</v>
+      <c r="A26" s="3">
+        <v>35796</v>
       </c>
       <c r="B26" s="1">
         <v>44700000000000</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>2.8400000000000002E-4</v>
       </c>
       <c r="D26">
@@ -1878,7 +1879,7 @@
       <c r="F26">
         <v>82278874</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26">
         <v>1.3899999999999999E-2</v>
       </c>
       <c r="H26">
@@ -1895,13 +1896,13 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1997</v>
+      <c r="A27" s="3">
+        <v>35431</v>
       </c>
       <c r="B27" s="1">
         <v>43500000000000</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>3.9500000000000001E-4</v>
       </c>
       <c r="D27">
@@ -1913,7 +1914,7 @@
       <c r="F27">
         <v>82732082</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27">
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="H27">
@@ -1930,13 +1931,13 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1996</v>
+      <c r="A28" s="3">
+        <v>35065</v>
       </c>
       <c r="B28" s="1">
         <v>41800000000000</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>3.5799999999999997E-4</v>
       </c>
       <c r="D28">
@@ -1948,7 +1949,7 @@
       <c r="F28">
         <v>83176752</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28">
         <v>1.44E-2</v>
       </c>
       <c r="H28">
@@ -1965,13 +1966,13 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1995</v>
+      <c r="A29" s="3">
+        <v>34700</v>
       </c>
       <c r="B29" s="1">
         <v>40400000000000</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>3.1E-4</v>
       </c>
       <c r="D29">
@@ -1983,7 +1984,7 @@
       <c r="F29">
         <v>83327727</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29">
         <v>1.47E-2</v>
       </c>
       <c r="H29">
@@ -2000,13 +2001,13 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1994</v>
+      <c r="A30" s="3">
+        <v>34335</v>
       </c>
       <c r="B30" s="1">
         <v>39200000000000</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>3.3399999999999999E-4</v>
       </c>
       <c r="D30">
@@ -2018,7 +2019,7 @@
       <c r="F30">
         <v>84006458</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H30">
@@ -2035,13 +2036,13 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1993</v>
+      <c r="A31" s="3">
+        <v>33970</v>
       </c>
       <c r="B31" s="1">
         <v>37900000000000</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>1.84E-4</v>
       </c>
       <c r="D31">
@@ -2053,7 +2054,7 @@
       <c r="F31">
         <v>85554981</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31">
         <v>1.55E-2</v>
       </c>
       <c r="H31">
@@ -2070,13 +2071,13 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1992</v>
+      <c r="A32" s="3">
+        <v>33604</v>
       </c>
       <c r="B32" s="1">
         <v>37200000000000</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>2.02E-4</v>
       </c>
       <c r="D32">
@@ -2088,7 +2089,7 @@
       <c r="F32">
         <v>87253925</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32">
         <v>1.61E-2</v>
       </c>
       <c r="H32">
@@ -2105,13 +2106,13 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1991</v>
+      <c r="A33" s="3">
+        <v>33239</v>
       </c>
       <c r="B33" s="1">
         <v>36500000000000</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>1.21E-4</v>
       </c>
       <c r="D33">
@@ -2123,7 +2124,7 @@
       <c r="F33">
         <v>90932781</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="H33">
@@ -2140,13 +2141,13 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1990</v>
+      <c r="A34" s="3">
+        <v>32874</v>
       </c>
       <c r="B34" s="1">
         <v>36100000000000</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>2.72E-4</v>
       </c>
       <c r="D34">
@@ -2158,7 +2159,7 @@
       <c r="F34">
         <v>93371378</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34">
         <v>1.78E-2</v>
       </c>
       <c r="H34">
@@ -2175,13 +2176,13 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1989</v>
+      <c r="A35" s="3">
+        <v>32509</v>
       </c>
       <c r="B35" s="1">
         <v>35100000000000</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>3.7199999999999999E-4</v>
       </c>
       <c r="D35">
@@ -2193,7 +2194,7 @@
       <c r="F35">
         <v>92439190</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H35">
@@ -2210,13 +2211,13 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1988</v>
+      <c r="A36" s="3">
+        <v>32143</v>
       </c>
       <c r="B36" s="1">
         <v>33800000000000</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>4.55E-4</v>
       </c>
       <c r="D36">
@@ -2228,7 +2229,7 @@
       <c r="F36">
         <v>92246145</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36">
         <v>1.83E-2</v>
       </c>
       <c r="H36">
@@ -2245,13 +2246,13 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1987</v>
+      <c r="A37" s="3">
+        <v>31778</v>
       </c>
       <c r="B37" s="1">
         <v>32400000000000</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>3.7500000000000001E-4</v>
       </c>
       <c r="D37">
@@ -2263,7 +2264,7 @@
       <c r="F37">
         <v>91673559</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="H37">
@@ -2280,13 +2281,13 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1986</v>
+      <c r="A38" s="3">
+        <v>31413</v>
       </c>
       <c r="B38" s="1">
         <v>31200000000000</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>3.2300000000000004E-4</v>
       </c>
       <c r="D38">
@@ -2298,7 +2299,7 @@
       <c r="F38">
         <v>89129373</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38">
         <v>1.83E-2</v>
       </c>
       <c r="H38">
@@ -2315,13 +2316,13 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1985</v>
+      <c r="A39" s="3">
+        <v>31048</v>
       </c>
       <c r="B39" s="1">
         <v>30200000000000</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>3.7100000000000002E-4</v>
       </c>
       <c r="D39">
@@ -2333,7 +2334,7 @@
       <c r="F39">
         <v>86767946</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39">
         <v>1.8100000000000002E-2</v>
       </c>
       <c r="H39">
@@ -2350,13 +2351,13 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1984</v>
+      <c r="A40" s="3">
+        <v>30682</v>
       </c>
       <c r="B40" s="1">
         <v>29100000000000</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>4.6799999999999999E-4</v>
       </c>
       <c r="D40">
@@ -2368,7 +2369,7 @@
       <c r="F40">
         <v>84847946</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40">
         <v>1.8100000000000002E-2</v>
       </c>
       <c r="H40">
@@ -2385,13 +2386,13 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1983</v>
+      <c r="A41" s="3">
+        <v>30317</v>
       </c>
       <c r="B41" s="1">
         <v>27800000000000</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>2.63E-4</v>
       </c>
       <c r="D41">
@@ -2403,7 +2404,7 @@
       <c r="F41">
         <v>84654152</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41">
         <v>1.84E-2</v>
       </c>
       <c r="H41">
@@ -2420,13 +2421,13 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1982</v>
+      <c r="A42" s="3">
+        <v>29952</v>
       </c>
       <c r="B42" s="1">
         <v>27100000000000</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>3.6000000000000001E-5</v>
       </c>
       <c r="D42">
@@ -2438,7 +2439,7 @@
       <c r="F42">
         <v>83896115</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="H42">
@@ -2455,13 +2456,13 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1981</v>
+      <c r="A43" s="3">
+        <v>29587</v>
       </c>
       <c r="B43" s="1">
         <v>27000000000000</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>1.94E-4</v>
       </c>
       <c r="D43">
@@ -2473,7 +2474,7 @@
       <c r="F43">
         <v>81171070</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43">
         <v>1.83E-2</v>
       </c>
       <c r="H43">
@@ -2490,13 +2491,13 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1980</v>
+      <c r="A44" s="3">
+        <v>29221</v>
       </c>
       <c r="B44" s="1">
         <v>26500000000000</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>1.8800000000000002E-4</v>
       </c>
       <c r="D44">
@@ -2508,7 +2509,7 @@
       <c r="F44">
         <v>79066708</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44">
         <v>1.8100000000000002E-2</v>
       </c>
       <c r="H44">
@@ -2525,13 +2526,13 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1979</v>
+      <c r="A45" s="3">
+        <v>28856</v>
       </c>
       <c r="B45" s="1">
         <v>26000000000000</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>4.1799999999999997E-4</v>
       </c>
       <c r="D45">
@@ -2543,7 +2544,7 @@
       <c r="F45">
         <v>76442026</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45">
         <v>1.78E-2</v>
       </c>
       <c r="H45">
@@ -2560,13 +2561,13 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1978</v>
+      <c r="A46" s="3">
+        <v>28491</v>
       </c>
       <c r="B46" s="1">
         <v>25000000000000</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>4.1599999999999997E-4</v>
       </c>
       <c r="D46">
@@ -2578,7 +2579,7 @@
       <c r="F46">
         <v>74233706</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46">
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="H46">
@@ -2595,13 +2596,13 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>1977</v>
+      <c r="A47" s="3">
+        <v>28126</v>
       </c>
       <c r="B47" s="1">
         <v>24000000000000</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>4.0099999999999999E-4</v>
       </c>
       <c r="D47">
@@ -2613,7 +2614,7 @@
       <c r="F47">
         <v>73617419</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47">
         <v>1.78E-2</v>
       </c>
       <c r="H47">

</xml_diff>